<commit_message>
[MOSIP-15491] Machine onboarding code made compatible with 1.1.5.4.
</commit_message>
<xml_diff>
--- a/deployment/v3/utils/onboard/machine/xlsx/machine.xlsx
+++ b/deployment/v3/utils/onboard/machine/xlsx/machine.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">language</t>
   </si>
   <si>
-    <t xml:space="preserve">Reg-Mach-1</t>
+    <t xml:space="preserve">desktop-fvgt677</t>
   </si>
   <si>
     <t xml:space="preserve">HighEnd</t>
@@ -202,18 +202,18 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="16.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="46.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.11"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[MOSIP-15491] Machine xls updated.
</commit_message>
<xml_diff>
--- a/deployment/v3/utils/onboard/machine/xlsx/machine.xlsx
+++ b/deployment/v3/utils/onboard/machine/xlsx/machine.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">MOR</t>
   </si>
   <si>
-    <t xml:space="preserve">MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp10M9v+R7xYWg1Mxgs7QIF6mO8wVY9ryRP066521L1UFZB1N8i2pNHhIEVwGln/BvV+uwpJlYO7fBS2ycDVWjhaHPHOe9sMosZiDnv0OoqcTGHTqD4zkqAPol/J3CvkrJZ1uQ7DK2G3OqgkjrnzFSBXIA9vh8b7pT/YSF+BKj9oc+T4oPqv5i/TvUIMBhImSIQhXT7kK5b71h25c2JZv+mrzV4kujt1O2nwFusmscWlYs/8KyKpTv3i6sXk/zO3uo+PT+pr/P6Lqyi9axOyBFysc3a1HB8xRchaSmFiXJnLPlD7E7r28KCDPhGaWyKtfkUBLfIDWQAFGUkriRD4YzwIDAQAB</t>
+    <t xml:space="preserve">MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAybUcwq1+HlGN53042d/EW0sQMjaooKvzhrQV0Lz/vk5tzR1w4ONIXlqKVai+JykUCrMgm57s1Qp4fHJBpU+IDGlezK6SamgT+o9wo8LpSinVN+7N2BwmZS28drc4Klr4YPE6sckf7VOqEdOf0uxetcBJZT5JkYih48Zj+XlKnT6kGRQtoUXf6tVLnc6UKyEosZEXx7awc8b/o6GGKqj4ruTHnzBZv/GUw1K/PgNZnWnXbQ8BcVQwb4hTONsV0eukBxwBhaMGA7PMrg4LLKP2VDebrkYzFm/eo5FwZRL7Syfa7M+JMzQwtToYG0yz1OjBXFMevi60paSfS9Lwm0FIHQIDAQAB</t>
   </si>
   <si>
     <t xml:space="preserve">eng</t>
@@ -201,8 +201,8 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[MOSIP-13637] Minor doc update.
</commit_message>
<xml_diff>
--- a/deployment/v3/utils/onboard/machine/xlsx/machine.xlsx
+++ b/deployment/v3/utils/onboard/machine/xlsx/machine.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t xml:space="preserve">fra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anusha-Lenovo-IdeaPad-S540-14IWL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAosTqynNYQj4mMZKcqcglyc2wLqHxNpnikcqhyt0sYF5To+X+gF1lZM5xKrOK25BuRILE3W0VmZSDcE5/XEposJ7CUdPLpKEVOqMsrjX7FC92YCd5wNWsn9sQeZHEZCLB0CTcjDfEjqf6+0Oi/cv1+ojMCUJ5NXddhMYiCseaYGgVED2lXYxqL5bqDH2j37sy7ckHGOPXDIvhs0YEbg+VEWXmAjQ4McVxQ/8sTYc+9E+zbEZngDW9w8SG7x60dGAjs7MCH63X3Lp0MwUl3QyQ8ysYuOMfvIO5NW2sU5SoMjUU5/WsJ8Vri61zyLLuuL/80T4ygPkorP34Gh+dTP0m7wIDAQAB</t>
   </si>
 </sst>
 </file>
@@ -149,7 +155,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -180,6 +186,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -202,18 +212,18 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="16.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="46.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.12"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -294,23 +304,57 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+    <row r="4" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>10001</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>365</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>10001</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>365</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>

</xml_diff>

<commit_message>
[MOSIP-16645] Updated for 1.2.0.
</commit_message>
<xml_diff>
--- a/deployment/v3/utils/onboard/machine/xlsx/machine.xlsx
+++ b/deployment/v3/utils/onboard/machine/xlsx/machine.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -43,9 +43,6 @@
     <t xml:space="preserve">valid_days</t>
   </si>
   <si>
-    <t xml:space="preserve">language</t>
-  </si>
-  <si>
     <t xml:space="preserve">desktop-fvgt677</t>
   </si>
   <si>
@@ -56,18 +53,6 @@
   </si>
   <si>
     <t xml:space="preserve">MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAybUcwq1+HlGN53042d/EW0sQMjaooKvzhrQV0Lz/vk5tzR1w4ONIXlqKVai+JykUCrMgm57s1Qp4fHJBpU+IDGlezK6SamgT+o9wo8LpSinVN+7N2BwmZS28drc4Klr4YPE6sckf7VOqEdOf0uxetcBJZT5JkYih48Zj+XlKnT6kGRQtoUXf6tVLnc6UKyEosZEXx7awc8b/o6GGKqj4ruTHnzBZv/GUw1K/PgNZnWnXbQ8BcVQwb4hTONsV0eukBxwBhaMGA7PMrg4LLKP2VDebrkYzFm/eo5FwZRL7Syfa7M+JMzQwtToYG0yz1OjBXFMevi60paSfS9Lwm0FIHQIDAQAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anusha-Lenovo-IdeaPad-S540-14IWL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAosTqynNYQj4mMZKcqcglyc2wLqHxNpnikcqhyt0sYF5To+X+gF1lZM5xKrOK25BuRILE3W0VmZSDcE5/XEposJ7CUdPLpKEVOqMsrjX7FC92YCd5wNWsn9sQeZHEZCLB0CTcjDfEjqf6+0Oi/cv1+ojMCUJ5NXddhMYiCseaYGgVED2lXYxqL5bqDH2j37sy7ckHGOPXDIvhs0YEbg+VEWXmAjQ4McVxQ/8sTYc+9E+zbEZngDW9w8SG7x60dGAjs7MCH63X3Lp0MwUl3QyQ8ysYuOMfvIO5NW2sU5SoMjUU5/WsJ8Vri61zyLLuuL/80T4ygPkorP34Gh+dTP0m7wIDAQAB</t>
   </si>
 </sst>
 </file>
@@ -155,7 +140,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,14 +167,6 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -209,13 +186,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="16.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.7"/>
@@ -223,7 +200,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="46.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,113 +225,57 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="27.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>10001</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="5" t="n">
         <v>365</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>10001</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>365</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>10001</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>365</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>10001</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>365</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
@@ -472,33 +393,6 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>